<commit_message>
Change Fungsional Scoring Criteria
</commit_message>
<xml_diff>
--- a/public/excels/TEMPLATE_PENILAIAN.xlsx
+++ b/public/excels/TEMPLATE_PENILAIAN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raysaki/Documents/Laravel/raudhah-akademik/public/excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{41D0076B-54B9-8A48-BF2B-710250F83B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C26799C-14E0-5840-AE8E-1C609A9FE2D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3260" windowWidth="28800" windowHeight="13440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3260" windowWidth="28800" windowHeight="13440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FUNGSIONAL" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>PENYAMPAIAN MATERI</t>
+          <t>KOMPETENSI PEDAGOGIK</t>
         </r>
       </text>
     </comment>
@@ -91,7 +91,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>PENGUASAAN MATERI DAN KELAS</t>
+          <t>KEHADIRAN MENGAJAR</t>
         </r>
       </text>
     </comment>
@@ -105,21 +105,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>KEHADIRAN MENGAJAR</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>ABSENSI MENGAJAR</t>
+          <t>INTEGRITAS</t>
         </r>
       </text>
     </comment>
@@ -274,7 +260,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
   <si>
     <t>NO</t>
   </si>
@@ -292,9 +278,6 @@
   </si>
   <si>
     <t>C3</t>
-  </si>
-  <si>
-    <t>C4</t>
   </si>
   <si>
     <t>KETERANGAN</t>
@@ -650,21 +633,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.1640625" customWidth="1"/>
     <col min="3" max="3" width="20.83203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="22.1640625" customWidth="1"/>
+    <col min="7" max="7" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="62" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -683,11 +666,8 @@
       <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -700,7 +680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
     </sheetView>
@@ -732,7 +712,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -770,13 +750,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>